<commit_message>
modify contoller for try cath issue
</commit_message>
<xml_diff>
--- a/Resources/TempFile/CustomerEntry.xlsx
+++ b/Resources/TempFile/CustomerEntry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahabub\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5C2798-E571-4D98-8A02-2513E4B3FE59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B2282F-E8B1-47E3-A753-A24ADC396E32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{F619B0D0-1591-4DC4-8A74-64D0B54EF623}"/>
   </bookViews>
@@ -31,42 +31,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Doctor</t>
+    <t>Chittagong</t>
   </si>
   <si>
-    <t>Driver</t>
+    <t>AbdullahAlMamun</t>
   </si>
   <si>
     <t>BusinessMan</t>
   </si>
   <si>
-    <t>Chittagong</t>
-  </si>
-  <si>
-    <t>illiterate</t>
-  </si>
-  <si>
-    <t>Dhaka</t>
-  </si>
-  <si>
-    <t>Khulna</t>
-  </si>
-  <si>
-    <t>BA</t>
-  </si>
-  <si>
-    <t>HSC</t>
-  </si>
-  <si>
-    <t>pppb775</t>
-  </si>
-  <si>
-    <t>opiuv</t>
-  </si>
-  <si>
-    <t>iofffgf</t>
+    <t>MA</t>
   </si>
 </sst>
 </file>
@@ -424,30 +400,32 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
     <col min="5" max="5" width="11.88671875" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>85000</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1">
-        <v>21000</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
       </c>
       <c r="F1">
         <v>25.369800000000001</v>
@@ -456,51 +434,9 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>15000</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <v>23.7835</v>
-      </c>
-      <c r="G2">
-        <v>13000</v>
-      </c>
-    </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>85000</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3">
-        <v>25.369800000000001</v>
-      </c>
-      <c r="G3">
-        <v>11000</v>
-      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H12" s="1"/>

</xml_diff>